<commit_message>
results, clustring and generation update
</commit_message>
<xml_diff>
--- a/Docs/Results/CUJ-CCT-P-18_02_25.xlsx
+++ b/Docs/Results/CUJ-CCT-P-18_02_25.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="RoBERTa" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="64">
   <si>
     <t>GPT2 - base</t>
   </si>
@@ -155,9 +155,6 @@
     <t>Templerun 2</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>TapFish</t>
   </si>
   <si>
@@ -176,27 +173,15 @@
     <t>BERTweet - base</t>
   </si>
   <si>
-    <t>RoBERTa + L + RC</t>
-  </si>
-  <si>
-    <t>BERTweet + L + RC</t>
-  </si>
-  <si>
     <t>Promedio</t>
   </si>
   <si>
-    <t>RoBERTa + L + RP</t>
-  </si>
-  <si>
     <t>RoBERTa + MLP + RC</t>
   </si>
   <si>
     <t>RoBERTa + MLP + RP</t>
   </si>
   <si>
-    <t>BERTweet + L + RP</t>
-  </si>
-  <si>
     <t>BERTweet + MLP + RC</t>
   </si>
   <si>
@@ -204,6 +189,39 @@
   </si>
   <si>
     <t>templerun2 (true)</t>
+  </si>
+  <si>
+    <t>Templerun 2 (SK)</t>
+  </si>
+  <si>
+    <t>templerun2 (SK)</t>
+  </si>
+  <si>
+    <t>RoBERTa + Linear + RC</t>
+  </si>
+  <si>
+    <t>RoBERTa + Linear + RP</t>
+  </si>
+  <si>
+    <t>BERTweet + Linear + RC</t>
+  </si>
+  <si>
+    <t>BERTweet + Linear + RP</t>
+  </si>
+  <si>
+    <t>: Mejora respecto al modelo original</t>
+  </si>
+  <si>
+    <t>: Decremento respecto al modelo original</t>
+  </si>
+  <si>
+    <t>: Experimento que falta por realizar</t>
+  </si>
+  <si>
+    <t>: Variante de ese modelo con mejores resultados en el dataset</t>
+  </si>
+  <si>
+    <t>: Variante de solución con mejores resultados en el dataset en general</t>
   </si>
 </sst>
 </file>
@@ -331,7 +349,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -769,19 +787,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -890,6 +895,80 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -901,7 +980,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1055,9 +1134,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1067,119 +1143,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="22" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="37" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="37" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="37" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="39" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="38" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1261,13 +1252,10 @@
     <xf numFmtId="165" fontId="4" fillId="3" borderId="13" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
@@ -1278,15 +1266,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1298,97 +1277,325 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="39" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="37" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="37" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="11" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="12" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="22" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="22" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="51" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="37" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="6" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="13" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="15" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="25" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="25" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="29" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="7" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="23" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="28" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="40" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="40" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="40" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="39" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
@@ -1710,7 +1917,7 @@
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="165" t="s">
+      <c r="B3" s="124" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -1728,10 +1935,10 @@
       <c r="G3" s="13">
         <v>0.91684434968017003</v>
       </c>
-      <c r="I3" s="176"/>
+      <c r="I3" s="114"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="166"/>
+      <c r="B4" s="125"/>
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
@@ -1747,10 +1954,10 @@
       <c r="G4" s="15">
         <v>0.93360160965794703</v>
       </c>
-      <c r="I4" s="176"/>
+      <c r="I4" s="114"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="166"/>
+      <c r="B5" s="125"/>
       <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
@@ -1766,10 +1973,10 @@
       <c r="G5" s="15">
         <v>0.94538606403013103</v>
       </c>
-      <c r="I5" s="176"/>
+      <c r="I5" s="114"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="166"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
@@ -1785,10 +1992,10 @@
       <c r="G6" s="15">
         <v>0.93006993006993</v>
       </c>
-      <c r="I6" s="176"/>
+      <c r="I6" s="114"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="166"/>
+      <c r="B7" s="125"/>
       <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
@@ -1804,10 +2011,10 @@
       <c r="G7" s="15">
         <v>0.92727272727272703</v>
       </c>
-      <c r="I7" s="176"/>
+      <c r="I7" s="114"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="167"/>
+      <c r="B8" s="126"/>
       <c r="C8" s="16" t="s">
         <v>6</v>
       </c>
@@ -1823,10 +2030,10 @@
       <c r="G8" s="18">
         <v>0.93063493614218096</v>
       </c>
-      <c r="I8" s="176"/>
+      <c r="I8" s="114"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="165" t="s">
+      <c r="B9" s="124" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -1852,7 +2059,7 @@
       <c r="N9" s="43"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="166"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="9" t="s">
         <v>2</v>
       </c>
@@ -1876,7 +2083,7 @@
       <c r="N10" s="43"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="166"/>
+      <c r="B11" s="125"/>
       <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
@@ -1900,7 +2107,7 @@
       <c r="N11" s="43"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="166"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="9" t="s">
         <v>4</v>
       </c>
@@ -1924,7 +2131,7 @@
       <c r="N12" s="47"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="166"/>
+      <c r="B13" s="125"/>
       <c r="C13" s="9" t="s">
         <v>5</v>
       </c>
@@ -1948,7 +2155,7 @@
       <c r="N13" s="43"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="167"/>
+      <c r="B14" s="126"/>
       <c r="C14" s="16" t="s">
         <v>6</v>
       </c>
@@ -1972,7 +2179,7 @@
       <c r="N14" s="43"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="124" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -1993,7 +2200,7 @@
       <c r="I15" s="44"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="166"/>
+      <c r="B16" s="125"/>
       <c r="C16" s="9" t="s">
         <v>2</v>
       </c>
@@ -2017,7 +2224,7 @@
       <c r="N16" s="43"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="166"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="9" t="s">
         <v>3</v>
       </c>
@@ -2041,7 +2248,7 @@
       <c r="N17" s="43"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="166"/>
+      <c r="B18" s="125"/>
       <c r="C18" s="9" t="s">
         <v>4</v>
       </c>
@@ -2065,7 +2272,7 @@
       <c r="N18" s="47"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="166"/>
+      <c r="B19" s="125"/>
       <c r="C19" s="9" t="s">
         <v>5</v>
       </c>
@@ -2083,7 +2290,7 @@
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="167"/>
+      <c r="B20" s="126"/>
       <c r="C20" s="16" t="s">
         <v>6</v>
       </c>
@@ -2101,7 +2308,7 @@
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="124" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -2121,7 +2328,7 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="166"/>
+      <c r="B22" s="125"/>
       <c r="C22" s="9" t="s">
         <v>2</v>
       </c>
@@ -2139,7 +2346,7 @@
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="166"/>
+      <c r="B23" s="125"/>
       <c r="C23" s="9" t="s">
         <v>3</v>
       </c>
@@ -2157,7 +2364,7 @@
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="166"/>
+      <c r="B24" s="125"/>
       <c r="C24" s="9" t="s">
         <v>4</v>
       </c>
@@ -2175,7 +2382,7 @@
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="166"/>
+      <c r="B25" s="125"/>
       <c r="C25" s="9" t="s">
         <v>5</v>
       </c>
@@ -2193,7 +2400,7 @@
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="167"/>
+      <c r="B26" s="126"/>
       <c r="C26" s="16" t="s">
         <v>6</v>
       </c>
@@ -2258,7 +2465,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="165" t="s">
+      <c r="B3" s="124" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -2278,7 +2485,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="166"/>
+      <c r="B4" s="125"/>
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
@@ -2296,7 +2503,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="166"/>
+      <c r="B5" s="125"/>
       <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
@@ -2314,7 +2521,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="166"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
@@ -2332,7 +2539,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="166"/>
+      <c r="B7" s="125"/>
       <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
@@ -2350,7 +2557,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="167"/>
+      <c r="B8" s="126"/>
       <c r="C8" s="16" t="s">
         <v>6</v>
       </c>
@@ -2368,7 +2575,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="165" t="s">
+      <c r="B9" s="124" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -2388,7 +2595,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="166"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="9" t="s">
         <v>2</v>
       </c>
@@ -2406,7 +2613,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="166"/>
+      <c r="B11" s="125"/>
       <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
@@ -2424,7 +2631,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="166"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="9" t="s">
         <v>4</v>
       </c>
@@ -2442,7 +2649,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="166"/>
+      <c r="B13" s="125"/>
       <c r="C13" s="9" t="s">
         <v>5</v>
       </c>
@@ -2460,7 +2667,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="167"/>
+      <c r="B14" s="126"/>
       <c r="C14" s="16" t="s">
         <v>6</v>
       </c>
@@ -2478,7 +2685,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="124" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -2498,7 +2705,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="166"/>
+      <c r="B16" s="125"/>
       <c r="C16" s="9" t="s">
         <v>2</v>
       </c>
@@ -2516,7 +2723,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="166"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="9" t="s">
         <v>3</v>
       </c>
@@ -2534,7 +2741,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="166"/>
+      <c r="B18" s="125"/>
       <c r="C18" s="9" t="s">
         <v>4</v>
       </c>
@@ -2552,7 +2759,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="166"/>
+      <c r="B19" s="125"/>
       <c r="C19" s="9" t="s">
         <v>5</v>
       </c>
@@ -2570,7 +2777,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="167"/>
+      <c r="B20" s="126"/>
       <c r="C20" s="16" t="s">
         <v>6</v>
       </c>
@@ -2588,7 +2795,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="124" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -2608,7 +2815,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="166"/>
+      <c r="B22" s="125"/>
       <c r="C22" s="9" t="s">
         <v>2</v>
       </c>
@@ -2626,7 +2833,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="166"/>
+      <c r="B23" s="125"/>
       <c r="C23" s="9" t="s">
         <v>3</v>
       </c>
@@ -2644,7 +2851,7 @@
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="166"/>
+      <c r="B24" s="125"/>
       <c r="C24" s="9" t="s">
         <v>4</v>
       </c>
@@ -2662,7 +2869,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="166"/>
+      <c r="B25" s="125"/>
       <c r="C25" s="9" t="s">
         <v>5</v>
       </c>
@@ -2680,7 +2887,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="167"/>
+      <c r="B26" s="126"/>
       <c r="C26" s="16" t="s">
         <v>6</v>
       </c>
@@ -2742,7 +2949,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="165" t="s">
+      <c r="B3" s="124" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -2762,7 +2969,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="166"/>
+      <c r="B4" s="125"/>
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
@@ -2780,7 +2987,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="166"/>
+      <c r="B5" s="125"/>
       <c r="C5" s="9" t="s">
         <v>3</v>
       </c>
@@ -2798,7 +3005,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="166"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
@@ -2816,7 +3023,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="166"/>
+      <c r="B7" s="125"/>
       <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
@@ -2834,7 +3041,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="167"/>
+      <c r="B8" s="126"/>
       <c r="C8" s="16" t="s">
         <v>6</v>
       </c>
@@ -2852,7 +3059,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="165" t="s">
+      <c r="B9" s="124" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -2872,7 +3079,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="166"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="9" t="s">
         <v>2</v>
       </c>
@@ -2890,7 +3097,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="166"/>
+      <c r="B11" s="125"/>
       <c r="C11" s="9" t="s">
         <v>3</v>
       </c>
@@ -2908,7 +3115,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="166"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="9" t="s">
         <v>4</v>
       </c>
@@ -2926,7 +3133,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="166"/>
+      <c r="B13" s="125"/>
       <c r="C13" s="9" t="s">
         <v>5</v>
       </c>
@@ -2944,7 +3151,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="167"/>
+      <c r="B14" s="126"/>
       <c r="C14" s="16" t="s">
         <v>6</v>
       </c>
@@ -2962,7 +3169,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="124" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -2982,7 +3189,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="166"/>
+      <c r="B16" s="125"/>
       <c r="C16" s="9" t="s">
         <v>2</v>
       </c>
@@ -3000,7 +3207,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="166"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="9" t="s">
         <v>3</v>
       </c>
@@ -3018,7 +3225,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="166"/>
+      <c r="B18" s="125"/>
       <c r="C18" s="9" t="s">
         <v>4</v>
       </c>
@@ -3036,7 +3243,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="166"/>
+      <c r="B19" s="125"/>
       <c r="C19" s="9" t="s">
         <v>5</v>
       </c>
@@ -3054,7 +3261,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="167"/>
+      <c r="B20" s="126"/>
       <c r="C20" s="16" t="s">
         <v>6</v>
       </c>
@@ -3072,7 +3279,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="124" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -3092,7 +3299,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="166"/>
+      <c r="B22" s="125"/>
       <c r="C22" s="9" t="s">
         <v>2</v>
       </c>
@@ -3110,7 +3317,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="166"/>
+      <c r="B23" s="125"/>
       <c r="C23" s="9" t="s">
         <v>3</v>
       </c>
@@ -3128,7 +3335,7 @@
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="166"/>
+      <c r="B24" s="125"/>
       <c r="C24" s="9" t="s">
         <v>4</v>
       </c>
@@ -3146,7 +3353,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="166"/>
+      <c r="B25" s="125"/>
       <c r="C25" s="9" t="s">
         <v>5</v>
       </c>
@@ -3164,7 +3371,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="167"/>
+      <c r="B26" s="126"/>
       <c r="C26" s="16" t="s">
         <v>6</v>
       </c>
@@ -3228,7 +3435,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="165" t="s">
+      <c r="B3" s="124" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="31" t="s">
@@ -3248,7 +3455,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="166"/>
+      <c r="B4" s="125"/>
       <c r="C4" s="32" t="s">
         <v>2</v>
       </c>
@@ -3266,7 +3473,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="166"/>
+      <c r="B5" s="125"/>
       <c r="C5" s="32" t="s">
         <v>3</v>
       </c>
@@ -3284,7 +3491,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="166"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="32" t="s">
         <v>4</v>
       </c>
@@ -3302,7 +3509,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="166"/>
+      <c r="B7" s="125"/>
       <c r="C7" s="32" t="s">
         <v>5</v>
       </c>
@@ -3320,7 +3527,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="167"/>
+      <c r="B8" s="126"/>
       <c r="C8" s="33" t="s">
         <v>6</v>
       </c>
@@ -3338,7 +3545,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="165" t="s">
+      <c r="B9" s="124" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="31" t="s">
@@ -3358,7 +3565,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="166"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="32" t="s">
         <v>2</v>
       </c>
@@ -3376,7 +3583,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="166"/>
+      <c r="B11" s="125"/>
       <c r="C11" s="32" t="s">
         <v>3</v>
       </c>
@@ -3394,7 +3601,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="166"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="32" t="s">
         <v>4</v>
       </c>
@@ -3412,7 +3619,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="166"/>
+      <c r="B13" s="125"/>
       <c r="C13" s="32" t="s">
         <v>5</v>
       </c>
@@ -3430,7 +3637,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="167"/>
+      <c r="B14" s="126"/>
       <c r="C14" s="16" t="s">
         <v>6</v>
       </c>
@@ -3448,7 +3655,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="124" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -3468,7 +3675,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="166"/>
+      <c r="B16" s="125"/>
       <c r="C16" s="9" t="s">
         <v>2</v>
       </c>
@@ -3486,7 +3693,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="166"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="9" t="s">
         <v>3</v>
       </c>
@@ -3504,7 +3711,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="166"/>
+      <c r="B18" s="125"/>
       <c r="C18" s="9" t="s">
         <v>4</v>
       </c>
@@ -3522,7 +3729,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="166"/>
+      <c r="B19" s="125"/>
       <c r="C19" s="9" t="s">
         <v>5</v>
       </c>
@@ -3540,7 +3747,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="167"/>
+      <c r="B20" s="126"/>
       <c r="C20" s="16" t="s">
         <v>6</v>
       </c>
@@ -3558,7 +3765,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="124" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -3578,7 +3785,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="166"/>
+      <c r="B22" s="125"/>
       <c r="C22" s="9" t="s">
         <v>2</v>
       </c>
@@ -3596,7 +3803,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="166"/>
+      <c r="B23" s="125"/>
       <c r="C23" s="9" t="s">
         <v>3</v>
       </c>
@@ -3614,7 +3821,7 @@
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="166"/>
+      <c r="B24" s="125"/>
       <c r="C24" s="9" t="s">
         <v>4</v>
       </c>
@@ -3632,7 +3839,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="166"/>
+      <c r="B25" s="125"/>
       <c r="C25" s="9" t="s">
         <v>5</v>
       </c>
@@ -3650,7 +3857,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="167"/>
+      <c r="B26" s="126"/>
       <c r="C26" s="16" t="s">
         <v>6</v>
       </c>
@@ -3668,8 +3875,8 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="165" t="s">
-        <v>57</v>
+      <c r="B27" s="124" t="s">
+        <v>52</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>1</v>
@@ -3688,7 +3895,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="166"/>
+      <c r="B28" s="125"/>
       <c r="C28" s="9" t="s">
         <v>2</v>
       </c>
@@ -3706,7 +3913,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="166"/>
+      <c r="B29" s="125"/>
       <c r="C29" s="9" t="s">
         <v>3</v>
       </c>
@@ -3724,7 +3931,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="166"/>
+      <c r="B30" s="125"/>
       <c r="C30" s="9" t="s">
         <v>4</v>
       </c>
@@ -3742,7 +3949,7 @@
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="166"/>
+      <c r="B31" s="125"/>
       <c r="C31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3760,7 +3967,7 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="167"/>
+      <c r="B32" s="126"/>
       <c r="C32" s="16" t="s">
         <v>6</v>
       </c>
@@ -3829,7 +4036,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="165" t="s">
+      <c r="B3" s="124" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="31" t="s">
@@ -3849,7 +4056,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="166"/>
+      <c r="B4" s="125"/>
       <c r="C4" s="32" t="s">
         <v>2</v>
       </c>
@@ -3867,7 +4074,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="166"/>
+      <c r="B5" s="125"/>
       <c r="C5" s="32" t="s">
         <v>3</v>
       </c>
@@ -3885,7 +4092,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="166"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="32" t="s">
         <v>4</v>
       </c>
@@ -3903,7 +4110,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="166"/>
+      <c r="B7" s="125"/>
       <c r="C7" s="32" t="s">
         <v>5</v>
       </c>
@@ -3921,7 +4128,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="167"/>
+      <c r="B8" s="126"/>
       <c r="C8" s="33" t="s">
         <v>6</v>
       </c>
@@ -3939,7 +4146,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="165" t="s">
+      <c r="B9" s="124" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="31" t="s">
@@ -3959,7 +4166,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="166"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="32" t="s">
         <v>2</v>
       </c>
@@ -3977,7 +4184,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="166"/>
+      <c r="B11" s="125"/>
       <c r="C11" s="32" t="s">
         <v>3</v>
       </c>
@@ -3995,7 +4202,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="166"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="32" t="s">
         <v>4</v>
       </c>
@@ -4013,7 +4220,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="166"/>
+      <c r="B13" s="125"/>
       <c r="C13" s="32" t="s">
         <v>5</v>
       </c>
@@ -4031,7 +4238,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="167"/>
+      <c r="B14" s="126"/>
       <c r="C14" s="33" t="s">
         <v>6</v>
       </c>
@@ -4049,7 +4256,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="124" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
@@ -4069,7 +4276,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="166"/>
+      <c r="B16" s="125"/>
       <c r="C16" s="9" t="s">
         <v>2</v>
       </c>
@@ -4087,7 +4294,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="166"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="9" t="s">
         <v>3</v>
       </c>
@@ -4105,7 +4312,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="166"/>
+      <c r="B18" s="125"/>
       <c r="C18" s="9" t="s">
         <v>4</v>
       </c>
@@ -4123,7 +4330,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="166"/>
+      <c r="B19" s="125"/>
       <c r="C19" s="9" t="s">
         <v>5</v>
       </c>
@@ -4141,7 +4348,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="167"/>
+      <c r="B20" s="126"/>
       <c r="C20" s="16" t="s">
         <v>6</v>
       </c>
@@ -4159,7 +4366,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="165" t="s">
+      <c r="B21" s="124" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -4179,7 +4386,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="166"/>
+      <c r="B22" s="125"/>
       <c r="C22" s="9" t="s">
         <v>2</v>
       </c>
@@ -4197,7 +4404,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="166"/>
+      <c r="B23" s="125"/>
       <c r="C23" s="9" t="s">
         <v>3</v>
       </c>
@@ -4215,7 +4422,7 @@
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="166"/>
+      <c r="B24" s="125"/>
       <c r="C24" s="9" t="s">
         <v>4</v>
       </c>
@@ -4233,7 +4440,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="166"/>
+      <c r="B25" s="125"/>
       <c r="C25" s="9" t="s">
         <v>5</v>
       </c>
@@ -4251,7 +4458,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="167"/>
+      <c r="B26" s="126"/>
       <c r="C26" s="16" t="s">
         <v>6</v>
       </c>
@@ -4282,16 +4489,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView topLeftCell="D31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="D28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="25.140625" customWidth="1"/>
@@ -4321,1429 +4528,1406 @@
       <c r="I2" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="56" t="s">
+      <c r="J2" s="55" t="s">
         <v>28</v>
       </c>
       <c r="K2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="L2" s="56" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="58" t="s">
+      <c r="N2" s="57" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="130" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="100">
+      <c r="D3" s="70">
         <v>0.9</v>
       </c>
-      <c r="E3" s="101">
+      <c r="E3" s="71">
         <v>0.90094443514209799</v>
       </c>
-      <c r="F3" s="100">
+      <c r="F3" s="70">
         <v>0.88038715428853698</v>
       </c>
-      <c r="G3" s="102">
+      <c r="G3" s="72">
         <v>0.88459075177312696</v>
       </c>
-      <c r="I3" s="168" t="s">
+      <c r="I3" s="127" t="s">
         <v>20</v>
       </c>
       <c r="J3" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="56">
+      <c r="K3" s="147">
         <v>0.93966666666666598</v>
       </c>
-      <c r="L3" s="60">
+      <c r="L3" s="148">
         <v>0.91014223876186096</v>
       </c>
-      <c r="M3" s="61">
+      <c r="M3" s="149">
         <v>0.95300145529521696</v>
       </c>
-      <c r="N3" s="62">
+      <c r="N3" s="150">
         <v>0.93063493614218096</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="172"/>
+      <c r="B4" s="131"/>
       <c r="C4" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="100">
+      <c r="D4" s="70">
         <v>0.84666666666666601</v>
       </c>
-      <c r="E4" s="101">
+      <c r="E4" s="71">
         <v>0.87769180929749602</v>
       </c>
-      <c r="F4" s="100">
+      <c r="F4" s="70">
         <v>0.80990058341481397</v>
       </c>
-      <c r="G4" s="102">
+      <c r="G4" s="72">
         <v>0.83597018030965797</v>
       </c>
-      <c r="I4" s="169"/>
-      <c r="J4" s="82" t="s">
+      <c r="I4" s="128"/>
+      <c r="J4" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="54">
+      <c r="K4" s="151">
         <v>0.94099999999999995</v>
       </c>
-      <c r="L4" s="51">
+      <c r="L4" s="152">
         <v>0.917067836705456</v>
       </c>
-      <c r="M4" s="49">
+      <c r="M4" s="153">
         <v>0.94982790027174702</v>
       </c>
-      <c r="N4" s="55">
+      <c r="N4" s="154">
         <v>0.93252228508214496</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="172"/>
+      <c r="B5" s="131"/>
       <c r="C5" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="103">
+      <c r="D5" s="73">
         <v>0.93766666666666598</v>
       </c>
-      <c r="E5" s="104">
+      <c r="E5" s="74">
         <v>0.919910936457637</v>
       </c>
-      <c r="F5" s="103">
+      <c r="F5" s="73">
         <v>0.94001077911094899</v>
       </c>
-      <c r="G5" s="105">
+      <c r="G5" s="75">
         <v>0.92966594521001</v>
       </c>
-      <c r="I5" s="169"/>
-      <c r="J5" s="78" t="s">
+      <c r="I5" s="128"/>
+      <c r="J5" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="49">
+      <c r="K5" s="153">
         <v>0.92999999999999905</v>
       </c>
-      <c r="L5" s="73">
+      <c r="L5" s="155">
         <v>0.90197634264710502</v>
       </c>
-      <c r="M5" s="49">
+      <c r="M5" s="153">
         <v>0.94261494199913598</v>
       </c>
-      <c r="N5" s="52">
+      <c r="N5" s="156">
         <v>0.91924775352578503</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="172"/>
+      <c r="B6" s="131"/>
       <c r="C6" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="103">
+      <c r="D6" s="73">
         <v>0.89833333333333298</v>
       </c>
-      <c r="E6" s="106">
+      <c r="E6" s="76">
         <v>0.86796611807933</v>
       </c>
-      <c r="F6" s="103">
+      <c r="F6" s="73">
         <v>0.904084815001713</v>
       </c>
-      <c r="G6" s="105">
+      <c r="G6" s="75">
         <v>0.88329708504354798</v>
       </c>
-      <c r="I6" s="169"/>
+      <c r="I6" s="128"/>
       <c r="J6" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="49">
+      <c r="K6" s="153">
         <v>0.93233333333333301</v>
       </c>
-      <c r="L6" s="51">
+      <c r="L6" s="152">
         <v>0.92440253992197297</v>
       </c>
-      <c r="M6" s="49">
+      <c r="M6" s="153">
         <v>0.92492408790908698</v>
       </c>
-      <c r="N6" s="52">
+      <c r="N6" s="156">
         <v>0.92403795172563097</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="173"/>
+      <c r="B7" s="132"/>
       <c r="C7" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="107">
+      <c r="D7" s="77">
         <v>0.93966666666666598</v>
       </c>
-      <c r="E7" s="108">
+      <c r="E7" s="78">
         <v>0.91014223876186096</v>
       </c>
-      <c r="F7" s="107">
+      <c r="F7" s="77">
         <v>0.95300145529521696</v>
       </c>
-      <c r="G7" s="109">
+      <c r="G7" s="79">
         <v>0.93063493614218096</v>
       </c>
-      <c r="I7" s="169"/>
+      <c r="I7" s="128"/>
       <c r="J7" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="49">
+      <c r="K7" s="153">
         <v>0.93099999999999905</v>
       </c>
-      <c r="L7" s="65">
+      <c r="L7" s="157">
         <v>0.94105892992615003</v>
       </c>
-      <c r="M7" s="49">
+      <c r="M7" s="153">
         <v>0.90957789395107302</v>
       </c>
-      <c r="N7" s="52">
+      <c r="N7" s="156">
         <v>0.92366895341794497</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="174" t="s">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="133" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="110">
+      <c r="D8" s="80">
         <v>0.74866666666666604</v>
       </c>
-      <c r="E8" s="111">
+      <c r="E8" s="81">
         <v>0.92345957678650203</v>
       </c>
-      <c r="F8" s="110">
+      <c r="F8" s="80">
         <v>0.76960898632406805</v>
       </c>
-      <c r="G8" s="112">
+      <c r="G8" s="82">
         <v>0.83784350915869898</v>
       </c>
-      <c r="I8" s="169"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="68"/>
+      <c r="I8" s="128"/>
+      <c r="J8" s="158" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="159">
+        <v>0.93766666666666598</v>
+      </c>
+      <c r="L8" s="160">
+        <v>0.919910936457637</v>
+      </c>
+      <c r="M8" s="159">
+        <v>0.94001077911094899</v>
+      </c>
+      <c r="N8" s="161">
+        <v>0.92966594521001</v>
+      </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="172"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="100">
+      <c r="D9" s="70">
         <v>0.86599999999999999</v>
       </c>
-      <c r="E9" s="101">
+      <c r="E9" s="71">
         <v>0.94493645994862596</v>
       </c>
-      <c r="F9" s="100">
+      <c r="F9" s="70">
         <v>0.87843464691931905</v>
       </c>
-      <c r="G9" s="102">
+      <c r="G9" s="72">
         <v>0.90930003916414903</v>
       </c>
-      <c r="I9" s="169"/>
-      <c r="J9" s="157" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="153">
-        <v>0.93766666666666598</v>
-      </c>
-      <c r="L9" s="70">
-        <v>0.919910936457637</v>
-      </c>
-      <c r="M9" s="153">
-        <v>0.94001077911094899</v>
+      <c r="I9" s="128"/>
+      <c r="J9" s="100" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="151">
+        <v>0.94199999999999895</v>
+      </c>
+      <c r="L9" s="155">
+        <v>0.91587328317245098</v>
+      </c>
+      <c r="M9" s="151">
+        <v>0.95263448409776297</v>
       </c>
       <c r="N9" s="154">
-        <v>0.92966594521001</v>
+        <v>0.93380756718922198</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="172"/>
+      <c r="B10" s="131"/>
       <c r="C10" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="113">
+      <c r="D10" s="83">
         <v>0.92466666666666597</v>
       </c>
-      <c r="E10" s="104">
+      <c r="E10" s="74">
         <v>0.97361925720361797</v>
       </c>
-      <c r="F10" s="103">
+      <c r="F10" s="73">
         <v>0.92401021848391895</v>
       </c>
-      <c r="G10" s="114">
+      <c r="G10" s="84">
         <v>0.94811172337970895</v>
       </c>
-      <c r="I10" s="169"/>
-      <c r="J10" s="131" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="54">
-        <v>0.94199999999999895</v>
-      </c>
-      <c r="L10" s="73">
-        <v>0.91587328317245098</v>
-      </c>
-      <c r="M10" s="54">
-        <v>0.95263448409776297</v>
-      </c>
-      <c r="N10" s="55">
-        <v>0.93380756718922198</v>
+      <c r="I10" s="128"/>
+      <c r="J10" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="153">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="L10" s="152">
+        <v>0.93341580994062701</v>
+      </c>
+      <c r="M10" s="153">
+        <v>0.92060523416489404</v>
+      </c>
+      <c r="N10" s="156">
+        <v>0.92540717681603002</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="172"/>
+      <c r="B11" s="131"/>
       <c r="C11" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="100">
+      <c r="D11" s="70">
         <v>0.84194444444444405</v>
       </c>
-      <c r="E11" s="101">
+      <c r="E11" s="71">
         <v>0.91269651582183398</v>
       </c>
-      <c r="F11" s="100">
+      <c r="F11" s="70">
         <v>0.88510628001188196</v>
       </c>
-      <c r="G11" s="102">
+      <c r="G11" s="72">
         <v>0.89287489814717602</v>
       </c>
-      <c r="I11" s="169"/>
-      <c r="J11" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11" s="49">
-        <v>0.93300000000000005</v>
-      </c>
-      <c r="L11" s="51">
-        <v>0.93341580994062701</v>
-      </c>
-      <c r="M11" s="49">
-        <v>0.92060523416489404</v>
-      </c>
-      <c r="N11" s="52">
-        <v>0.92540717681603002</v>
+      <c r="I11" s="128"/>
+      <c r="J11" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="153">
+        <v>0.92266666666666597</v>
+      </c>
+      <c r="L11" s="155">
+        <v>0.90100146539409598</v>
+      </c>
+      <c r="M11" s="153">
+        <v>0.92828697469414001</v>
+      </c>
+      <c r="N11" s="156">
+        <v>0.91222117035461403</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="175"/>
+      <c r="B12" s="134"/>
       <c r="C12" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="115">
+      <c r="D12" s="85">
         <v>0.92166666666666597</v>
       </c>
-      <c r="E12" s="108">
+      <c r="E12" s="78">
         <v>0.945716164152685</v>
       </c>
-      <c r="F12" s="107">
+      <c r="F12" s="77">
         <v>0.94535122342216804</v>
       </c>
-      <c r="G12" s="116">
+      <c r="G12" s="86">
         <v>0.94455614281048605</v>
       </c>
-      <c r="I12" s="169"/>
-      <c r="J12" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" s="49">
-        <v>0.92266666666666597</v>
-      </c>
-      <c r="L12" s="73">
-        <v>0.90100146539409598</v>
-      </c>
-      <c r="M12" s="49">
-        <v>0.92828697469414001</v>
-      </c>
-      <c r="N12" s="52">
-        <v>0.91222117035461403</v>
+      <c r="I12" s="129"/>
+      <c r="J12" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="162">
+        <v>0.93399999999999905</v>
+      </c>
+      <c r="L12" s="163">
+        <v>0.93313224206713596</v>
+      </c>
+      <c r="M12" s="162">
+        <v>0.92130705026925197</v>
+      </c>
+      <c r="N12" s="164">
+        <v>0.926820944877769</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="174" t="s">
+      <c r="B13" s="133" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="117">
+      <c r="D13" s="87">
         <v>0.90433333333333299</v>
       </c>
-      <c r="E13" s="118">
+      <c r="E13" s="88">
         <v>0.774176426721637</v>
       </c>
-      <c r="F13" s="117">
+      <c r="F13" s="87">
         <v>0.87694181049036202</v>
       </c>
-      <c r="G13" s="119">
+      <c r="G13" s="89">
         <v>0.81655865710653197</v>
       </c>
-      <c r="I13" s="169"/>
-      <c r="J13" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="K13" s="49">
-        <v>0.93399999999999905</v>
-      </c>
-      <c r="L13" s="51">
-        <v>0.93313224206713596</v>
-      </c>
-      <c r="M13" s="49">
-        <v>0.92130705026925197</v>
-      </c>
-      <c r="N13" s="52">
-        <v>0.926820944877769</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="172"/>
+      <c r="I13" s="127" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="165">
+        <v>0.92166666666666597</v>
+      </c>
+      <c r="L13" s="147">
+        <v>0.945716164152685</v>
+      </c>
+      <c r="M13" s="147">
+        <v>0.94535122342216804</v>
+      </c>
+      <c r="N13" s="150">
+        <v>0.94455614281048605</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="131"/>
       <c r="C14" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="103">
+      <c r="D14" s="73">
         <v>0.88633333333333297</v>
       </c>
-      <c r="E14" s="120">
+      <c r="E14" s="90">
         <v>0.95775427798383295</v>
       </c>
-      <c r="F14" s="103">
+      <c r="F14" s="73">
         <v>0.89999245790198301</v>
       </c>
-      <c r="G14" s="105">
+      <c r="G14" s="75">
         <v>0.92715192147623104</v>
       </c>
-      <c r="I14" s="169"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="70"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="69"/>
+      <c r="I14" s="128"/>
+      <c r="J14" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" s="166">
+        <v>0.91066666666666596</v>
+      </c>
+      <c r="L14" s="153">
+        <v>0.942167817193996</v>
+      </c>
+      <c r="M14" s="153">
+        <v>0.93275866437296595</v>
+      </c>
+      <c r="N14" s="156">
+        <v>0.93693594016009696</v>
+      </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="172"/>
+      <c r="B15" s="131"/>
       <c r="C15" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="113">
+      <c r="D15" s="83">
         <v>0.94133333333333302</v>
       </c>
-      <c r="E15" s="106">
+      <c r="E15" s="76">
         <v>0.94691356441715102</v>
       </c>
-      <c r="F15" s="103">
+      <c r="F15" s="73">
         <v>0.97502493880587304</v>
       </c>
-      <c r="G15" s="114">
+      <c r="G15" s="84">
         <v>0.960488422521524</v>
       </c>
-      <c r="I15" s="168" t="s">
-        <v>38</v>
-      </c>
-      <c r="J15" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="K15" s="75">
-        <v>0.92166666666666597</v>
-      </c>
-      <c r="L15" s="56">
-        <v>0.945716164152685</v>
-      </c>
-      <c r="M15" s="56">
-        <v>0.94535122342216804</v>
-      </c>
-      <c r="N15" s="62">
-        <v>0.94455614281048605</v>
+      <c r="I15" s="128"/>
+      <c r="J15" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="167">
+        <v>0.92666666666666597</v>
+      </c>
+      <c r="L15" s="151">
+        <v>0.95597680512565897</v>
+      </c>
+      <c r="M15" s="153">
+        <v>0.941515641019397</v>
+      </c>
+      <c r="N15" s="154">
+        <v>0.94852841904531404</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="172"/>
+      <c r="B16" s="131"/>
       <c r="C16" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="100">
+      <c r="D16" s="70">
         <v>0.81099999999999905</v>
       </c>
-      <c r="E16" s="121">
+      <c r="E16" s="91">
         <v>0.96026319319002196</v>
       </c>
-      <c r="F16" s="100">
+      <c r="F16" s="70">
         <v>0.82422861255630198</v>
       </c>
-      <c r="G16" s="102">
+      <c r="G16" s="72">
         <v>0.88515109211177201</v>
       </c>
-      <c r="I16" s="169"/>
+      <c r="I16" s="128"/>
       <c r="J16" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="K16" s="79">
-        <v>0.91066666666666596</v>
-      </c>
-      <c r="L16" s="49">
-        <v>0.942167817193996</v>
-      </c>
-      <c r="M16" s="49">
-        <v>0.93275866437296595</v>
-      </c>
-      <c r="N16" s="52">
-        <v>0.93693594016009696</v>
+        <v>31</v>
+      </c>
+      <c r="K16" s="166">
+        <v>0.91666666666666596</v>
+      </c>
+      <c r="L16" s="153">
+        <v>0.90975759748395801</v>
+      </c>
+      <c r="M16" s="151">
+        <v>0.97104605001272204</v>
+      </c>
+      <c r="N16" s="156">
+        <v>0.93904052682102801</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="175"/>
+      <c r="B17" s="134"/>
       <c r="C17" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="122">
+      <c r="D17" s="92">
         <v>0.92733333333333301</v>
       </c>
-      <c r="E17" s="123">
+      <c r="E17" s="93">
         <v>0.92236003297696201</v>
       </c>
-      <c r="F17" s="124">
+      <c r="F17" s="94">
         <v>0.98012209968247499</v>
       </c>
-      <c r="G17" s="125">
+      <c r="G17" s="95">
         <v>0.94960659490389299</v>
       </c>
-      <c r="I17" s="169"/>
-      <c r="J17" s="130" t="s">
-        <v>33</v>
-      </c>
-      <c r="K17" s="80">
-        <v>0.92666666666666597</v>
-      </c>
-      <c r="L17" s="54">
-        <v>0.95597680512565897</v>
-      </c>
-      <c r="M17" s="49">
-        <v>0.941515641019397</v>
-      </c>
-      <c r="N17" s="55">
-        <v>0.94852841904531404</v>
+      <c r="I17" s="128"/>
+      <c r="J17" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" s="168">
+        <v>0.92366666666666597</v>
+      </c>
+      <c r="L17" s="138">
+        <v>0.94668176595108799</v>
+      </c>
+      <c r="M17" s="138">
+        <v>0.94592810163707497</v>
+      </c>
+      <c r="N17" s="169">
+        <v>0.94611855796508304</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="174" t="s">
+      <c r="B18" s="133" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="103">
+      <c r="D18" s="73">
         <v>0.89800000000000002</v>
       </c>
-      <c r="E18" s="106">
+      <c r="E18" s="76">
         <v>0.83380446160172395</v>
       </c>
-      <c r="F18" s="103">
+      <c r="F18" s="73">
         <v>0.822946213095609</v>
       </c>
-      <c r="G18" s="105">
-        <v>0.82443696037685399</v>
-      </c>
-      <c r="I18" s="169"/>
-      <c r="J18" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="K18" s="79">
-        <v>0.91666666666666596</v>
-      </c>
-      <c r="L18" s="49">
-        <v>0.90975759748395801</v>
-      </c>
-      <c r="M18" s="54">
-        <v>0.97104605001272204</v>
-      </c>
-      <c r="N18" s="52">
-        <v>0.93904052682102801</v>
+      <c r="G18" s="145"/>
+      <c r="I18" s="128"/>
+      <c r="J18" s="170" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="171">
+        <v>0.92466666666666597</v>
+      </c>
+      <c r="L18" s="172">
+        <v>0.97361925720361797</v>
+      </c>
+      <c r="M18" s="173">
+        <v>0.92401021848391895</v>
+      </c>
+      <c r="N18" s="174">
+        <v>0.94811172337970895</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="172"/>
+      <c r="B19" s="131"/>
       <c r="C19" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="103">
+      <c r="D19" s="73">
         <v>0.83599999999999997</v>
       </c>
-      <c r="E19" s="106">
+      <c r="E19" s="76">
         <v>0.88455725174062005</v>
       </c>
-      <c r="F19" s="103">
+      <c r="F19" s="73">
         <v>0.88943449794617901</v>
       </c>
-      <c r="G19" s="105">
-        <v>0.88272122487528404</v>
-      </c>
-      <c r="I19" s="169"/>
-      <c r="J19" s="86" t="s">
-        <v>32</v>
-      </c>
-      <c r="K19" s="77">
-        <v>0.92366666666666597</v>
-      </c>
-      <c r="L19" s="63">
-        <v>0.94668176595108799</v>
-      </c>
-      <c r="M19" s="63">
-        <v>0.94592810163707497</v>
-      </c>
-      <c r="N19" s="64">
-        <v>0.94611855796508304</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="172"/>
+      <c r="G19" s="145"/>
+      <c r="I19" s="128"/>
+      <c r="J19" s="100" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" s="167">
+        <v>0.93133333333333301</v>
+      </c>
+      <c r="L19" s="153">
+        <v>0.95379757378877705</v>
+      </c>
+      <c r="M19" s="138">
+        <v>0.949377770720088</v>
+      </c>
+      <c r="N19" s="154">
+        <v>0.95153501290619003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="131"/>
       <c r="C20" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="113">
+      <c r="D20" s="83">
         <v>0.93200000000000005</v>
       </c>
-      <c r="E20" s="106">
+      <c r="E20" s="76">
         <v>0.94774151470795298</v>
       </c>
-      <c r="F20" s="113">
+      <c r="F20" s="83">
         <v>0.95603291396641799</v>
       </c>
-      <c r="G20" s="114">
-        <v>0.95167123552427801</v>
-      </c>
-      <c r="I20" s="169"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="76"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="72"/>
-      <c r="N20" s="69"/>
+      <c r="G20" s="84">
+        <v>0.95655542267451998</v>
+      </c>
+      <c r="I20" s="128"/>
+      <c r="J20" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="166">
+        <v>0.92333333333333301</v>
+      </c>
+      <c r="L20" s="153">
+        <v>0.924701882211309</v>
+      </c>
+      <c r="M20" s="151">
+        <v>0.96527041881140796</v>
+      </c>
+      <c r="N20" s="156">
+        <v>0.94430969519343799</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="172"/>
+      <c r="B21" s="131"/>
       <c r="C21" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="100">
+      <c r="D21" s="70">
         <v>0.81399999999999995</v>
       </c>
-      <c r="E21" s="101">
+      <c r="E21" s="71">
         <v>0.93529471319514301</v>
       </c>
-      <c r="F21" s="100">
+      <c r="F21" s="70">
         <v>0.84111573320072097</v>
       </c>
-      <c r="G21" s="102">
-        <v>0.87920035047497902</v>
-      </c>
-      <c r="I21" s="169"/>
-      <c r="J21" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="K21" s="75">
-        <v>0.92466666666666597</v>
-      </c>
-      <c r="L21" s="61">
-        <v>0.97361925720361797</v>
-      </c>
-      <c r="M21" s="56">
-        <v>0.92401021848391895</v>
-      </c>
-      <c r="N21" s="62">
-        <v>0.94811172337970895</v>
+      <c r="G21" s="146"/>
+      <c r="I21" s="128"/>
+      <c r="J21" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" s="168">
+        <v>0.92799999999999905</v>
+      </c>
+      <c r="L21" s="153">
+        <v>0.94979883849881896</v>
+      </c>
+      <c r="M21" s="175">
+        <v>0.94950331977266</v>
+      </c>
+      <c r="N21" s="169">
+        <v>0.949132760189906</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="175"/>
+      <c r="B22" s="134"/>
       <c r="C22" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="122">
+      <c r="D22" s="92">
         <v>0.91366666666666596</v>
       </c>
-      <c r="E22" s="126">
+      <c r="E22" s="96">
         <v>0.95814644463200904</v>
       </c>
-      <c r="F22" s="122">
+      <c r="F22" s="92">
         <v>0.92440880347615895</v>
       </c>
-      <c r="G22" s="125">
-        <v>0.94032543064146701</v>
-      </c>
-      <c r="I22" s="169"/>
-      <c r="J22" s="131" t="s">
-        <v>37</v>
-      </c>
-      <c r="K22" s="80">
-        <v>0.93133333333333301</v>
-      </c>
-      <c r="L22" s="49">
-        <v>0.95379757378877705</v>
-      </c>
-      <c r="M22" s="63">
-        <v>0.949377770720088</v>
-      </c>
-      <c r="N22" s="55">
-        <v>0.95153501290619003</v>
+      <c r="G22" s="95">
+        <v>0.95037693946635804</v>
+      </c>
+      <c r="I22" s="129"/>
+      <c r="J22" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22" s="176">
+        <v>0.878</v>
+      </c>
+      <c r="L22" s="162">
+        <v>0.908083775232572</v>
+      </c>
+      <c r="M22" s="177">
+        <v>0.92680206383419494</v>
+      </c>
+      <c r="N22" s="164">
+        <v>0.91524186903115701</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I23" s="169"/>
-      <c r="J23" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="K23" s="79">
-        <v>0.92333333333333301</v>
-      </c>
-      <c r="L23" s="49">
-        <v>0.924701882211309</v>
-      </c>
-      <c r="M23" s="54">
-        <v>0.96527041881140796</v>
-      </c>
-      <c r="N23" s="52">
-        <v>0.94430969519343799</v>
+      <c r="I23" s="127" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" s="147">
+        <v>0.92733333333333301</v>
+      </c>
+      <c r="L23" s="148">
+        <v>0.92236003297696201</v>
+      </c>
+      <c r="M23" s="147">
+        <v>0.98012209968247499</v>
+      </c>
+      <c r="N23" s="178">
+        <v>0.94960659490389299</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I24" s="169"/>
-      <c r="J24" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="K24" s="77">
-        <v>0.92799999999999905</v>
-      </c>
-      <c r="L24" s="49">
-        <v>0.94979883849881896</v>
-      </c>
-      <c r="M24" s="127">
-        <v>0.94950331977266</v>
-      </c>
-      <c r="N24" s="64">
-        <v>0.949132760189906</v>
+      <c r="I24" s="128"/>
+      <c r="J24" s="62" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="151">
+        <v>0.93466666666666598</v>
+      </c>
+      <c r="L24" s="152">
+        <v>0.931014491990101</v>
+      </c>
+      <c r="M24" s="151">
+        <v>0.98138206994140098</v>
+      </c>
+      <c r="N24" s="179">
+        <v>0.95550025542346095</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I25" s="169"/>
-      <c r="J25" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="K25" s="79">
-        <v>0.878</v>
-      </c>
-      <c r="L25" s="49">
-        <v>0.908083775232572</v>
-      </c>
-      <c r="M25" s="63">
-        <v>0.92680206383419494</v>
-      </c>
-      <c r="N25" s="52">
-        <v>0.91524186903115701</v>
+      <c r="I25" s="128"/>
+      <c r="J25" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="138">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="L25" s="152">
+        <v>0.93683604128367404</v>
+      </c>
+      <c r="M25" s="153">
+        <v>0.96729452452223497</v>
+      </c>
+      <c r="N25" s="123">
+        <v>0.95137752291535904</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="129" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="144" t="s">
+      <c r="B26" s="98" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="143" t="s">
+      <c r="D26" s="109" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="144" t="s">
+      <c r="E26" s="110" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="109" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="143" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" s="145" t="s">
-        <v>50</v>
-      </c>
-      <c r="I26" s="170"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="76"/>
-      <c r="L26" s="81"/>
-      <c r="M26" s="81"/>
-      <c r="N26" s="69"/>
+      <c r="G26" s="111" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" s="128"/>
+      <c r="J26" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="K26" s="153">
+        <v>0.90933333333333299</v>
+      </c>
+      <c r="L26" s="157">
+        <v>0.96713560522742703</v>
+      </c>
+      <c r="M26" s="153">
+        <v>0.91986275215338198</v>
+      </c>
+      <c r="N26" s="139">
+        <v>0.94181503831139002</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
-      <c r="B27" s="141" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="70">
+      <c r="B27" s="107" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="197">
         <v>0.88459075177312696</v>
       </c>
-      <c r="D27" s="136">
+      <c r="D27" s="147">
         <v>0.83784350915869898</v>
       </c>
-      <c r="E27" s="70">
+      <c r="E27" s="148">
         <v>0.81655865710653197</v>
       </c>
-      <c r="F27" s="136">
-        <v>0.82443696037685399</v>
-      </c>
-      <c r="G27" s="69">
+      <c r="F27" s="198"/>
+      <c r="G27" s="150">
         <f>AVERAGE(C27,D27,E27,F27)</f>
-        <v>0.84085746960380292</v>
-      </c>
-      <c r="I27" s="168" t="s">
-        <v>39</v>
-      </c>
-      <c r="J27" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="K27" s="56">
-        <v>0.92733333333333301</v>
-      </c>
-      <c r="L27" s="60">
-        <v>0.92236003297696201</v>
-      </c>
-      <c r="M27" s="56">
-        <v>0.98012209968247499</v>
-      </c>
-      <c r="N27" s="84">
-        <v>0.94960659490389299</v>
+        <v>0.84633097267945256</v>
+      </c>
+      <c r="I27" s="128"/>
+      <c r="J27" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="K27" s="138">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="L27" s="152">
+        <v>0.93961149233746</v>
+      </c>
+      <c r="M27" s="153">
+        <v>0.97126867113695903</v>
+      </c>
+      <c r="N27" s="123">
+        <v>0.95498447463069402</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
-      <c r="B28" s="141" t="s">
+      <c r="B28" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="70">
+      <c r="C28" s="199">
         <v>0.88329708504354798</v>
       </c>
-      <c r="D28" s="136">
+      <c r="D28" s="200">
         <v>0.89287489814717602</v>
       </c>
-      <c r="E28" s="70">
+      <c r="E28" s="201">
         <v>0.88515109211177201</v>
       </c>
-      <c r="F28" s="136">
-        <v>0.87920035047497902</v>
-      </c>
-      <c r="G28" s="69">
-        <f t="shared" ref="G28:G30" si="0">AVERAGE(C28,D28,E28,F28)</f>
-        <v>0.88513085644436873</v>
-      </c>
-      <c r="I28" s="169"/>
-      <c r="J28" s="82" t="s">
-        <v>30</v>
-      </c>
-      <c r="K28" s="54">
-        <v>0.93466666666666598</v>
-      </c>
-      <c r="L28" s="51">
-        <v>0.931014491990101</v>
-      </c>
-      <c r="M28" s="54">
-        <v>0.98138206994140098</v>
-      </c>
-      <c r="N28" s="91">
-        <v>0.95550025542346095</v>
+      <c r="F28" s="183"/>
+      <c r="G28" s="202">
+        <f>AVERAGE(C28,D28,E28,F28)</f>
+        <v>0.88710769176749871</v>
+      </c>
+      <c r="I28" s="128"/>
+      <c r="J28" s="170" t="s">
+        <v>24</v>
+      </c>
+      <c r="K28" s="173">
+        <v>0.94133333333333302</v>
+      </c>
+      <c r="L28" s="160">
+        <v>0.94691356441715102</v>
+      </c>
+      <c r="M28" s="173">
+        <v>0.97502493880587304</v>
+      </c>
+      <c r="N28" s="180">
+        <v>0.960488422521524</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
-      <c r="B29" s="141" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="70">
+      <c r="B29" s="107" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="199">
         <v>0.83597018030965797</v>
       </c>
-      <c r="D29" s="136">
+      <c r="D29" s="200">
         <v>0.90930003916414903</v>
       </c>
-      <c r="E29" s="70">
+      <c r="E29" s="201">
         <v>0.92715192147623104</v>
       </c>
-      <c r="F29" s="136">
-        <v>0.88272122487528404</v>
-      </c>
-      <c r="G29" s="69">
-        <f t="shared" si="0"/>
-        <v>0.88878584145633055</v>
-      </c>
-      <c r="I29" s="169"/>
-      <c r="J29" s="78" t="s">
-        <v>33</v>
-      </c>
-      <c r="K29" s="63">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="L29" s="51">
-        <v>0.93683604128367404</v>
-      </c>
-      <c r="M29" s="49">
-        <v>0.96729452452223497</v>
-      </c>
-      <c r="N29" s="89">
-        <v>0.95137752291535904</v>
+      <c r="F29" s="183"/>
+      <c r="G29" s="202">
+        <f>AVERAGE(C29,D29,E29,F29)</f>
+        <v>0.89080738031667928</v>
+      </c>
+      <c r="I29" s="128"/>
+      <c r="J29" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" s="153">
+        <v>0.93933333333333302</v>
+      </c>
+      <c r="L29" s="152">
+        <v>0.96355346670985098</v>
+      </c>
+      <c r="M29" s="153">
+        <v>0.95749652547193698</v>
+      </c>
+      <c r="N29" s="139">
+        <v>0.96009563221816197</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4</v>
       </c>
-      <c r="B30" s="148" t="s">
+      <c r="B30" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="146">
+      <c r="C30" s="203">
         <v>0.93063493614218096</v>
       </c>
-      <c r="D30" s="135">
+      <c r="D30" s="173">
         <v>0.94455614281048605</v>
       </c>
-      <c r="E30" s="146">
+      <c r="E30" s="160">
         <v>0.94960659490389299</v>
       </c>
-      <c r="F30" s="135">
-        <v>0.94032543064146701</v>
-      </c>
-      <c r="G30" s="149">
-        <f t="shared" si="0"/>
-        <v>0.94128077612450678</v>
-      </c>
-      <c r="I30" s="169"/>
-      <c r="J30" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="K30" s="49">
-        <v>0.90933333333333299</v>
-      </c>
-      <c r="L30" s="65">
-        <v>0.96713560522742703</v>
-      </c>
-      <c r="M30" s="49">
-        <v>0.91986275215338198</v>
-      </c>
-      <c r="N30" s="88">
-        <v>0.94181503831139002</v>
+      <c r="F30" s="173">
+        <v>0.95037693946635804</v>
+      </c>
+      <c r="G30" s="174">
+        <f>AVERAGE(C30,D30,E30,F30)</f>
+        <v>0.94379365333072951</v>
+      </c>
+      <c r="I30" s="128"/>
+      <c r="J30" s="181" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" s="151">
+        <v>0.94333333333333302</v>
+      </c>
+      <c r="L30" s="157">
+        <v>0.96939454421520399</v>
+      </c>
+      <c r="M30" s="153">
+        <v>0.95635467660047002</v>
+      </c>
+      <c r="N30" s="179">
+        <v>0.962621751359374</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5</v>
       </c>
-      <c r="B31" s="141" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="156">
+      <c r="B31" s="107" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="204">
         <v>0.93252228508214496</v>
       </c>
-      <c r="D31" s="136">
-        <v>0.92695667228769496</v>
-      </c>
-      <c r="E31" s="70">
+      <c r="D31" s="153">
+        <v>0.93693594016009696</v>
+      </c>
+      <c r="E31" s="152">
         <v>0.95550025542346095</v>
       </c>
-      <c r="F31" s="136">
-        <v>0.94621159827797796</v>
-      </c>
-      <c r="G31" s="69">
-        <f t="shared" ref="G31:G34" si="1">AVERAGE(C31,D31,E31,F31)</f>
-        <v>0.94029770276781965</v>
-      </c>
-      <c r="I31" s="169"/>
+      <c r="F31" s="138">
+        <v>0.95050627178595104</v>
+      </c>
+      <c r="G31" s="202">
+        <f>AVERAGE(C31,D31,E31,F31)</f>
+        <v>0.94386618811291345</v>
+      </c>
+      <c r="I31" s="128"/>
       <c r="J31" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="K31" s="63">
-        <v>0.93333333333333302</v>
-      </c>
-      <c r="L31" s="51">
-        <v>0.93961149233746</v>
-      </c>
-      <c r="M31" s="49">
-        <v>0.97126867113695903</v>
-      </c>
-      <c r="N31" s="89">
-        <v>0.95498447463069402</v>
+        <v>35</v>
+      </c>
+      <c r="K31" s="138">
+        <v>0.94133333333333302</v>
+      </c>
+      <c r="L31" s="155">
+        <v>0.94269821780582097</v>
+      </c>
+      <c r="M31" s="151">
+        <v>0.97861716312371705</v>
+      </c>
+      <c r="N31" s="139">
+        <v>0.96020358147077001</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>6</v>
       </c>
-      <c r="B32" s="139" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="70">
+      <c r="B32" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="205">
         <v>0.91924775352578503</v>
       </c>
-      <c r="D32" s="136">
-        <v>0.93693594016009696</v>
-      </c>
-      <c r="E32" s="70">
+      <c r="D32" s="138">
+        <v>0.94852841904531404</v>
+      </c>
+      <c r="E32" s="152">
         <v>0.95137752291535904</v>
       </c>
-      <c r="F32" s="136">
-        <v>0.94265481086242897</v>
-      </c>
-      <c r="G32" s="69">
-        <f t="shared" si="1"/>
-        <v>0.9375540068659175</v>
-      </c>
-      <c r="I32" s="169"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="81"/>
-      <c r="L32" s="70"/>
-      <c r="M32" s="81"/>
-      <c r="N32" s="87"/>
+      <c r="F32" s="138">
+        <v>0.95081201999177301</v>
+      </c>
+      <c r="G32" s="202">
+        <f>AVERAGE(C32,D32,E32,F32)</f>
+        <v>0.94249142886955783</v>
+      </c>
+      <c r="I32" s="129"/>
+      <c r="J32" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="K32" s="153">
+        <v>0.93333333333333302</v>
+      </c>
+      <c r="L32" s="152">
+        <v>0.952397096873424</v>
+      </c>
+      <c r="M32" s="153">
+        <v>0.96002205787604</v>
+      </c>
+      <c r="N32" s="139">
+        <v>0.95568813273184805</v>
+      </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7</v>
       </c>
-      <c r="B33" s="139" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="70">
+      <c r="B33" s="105" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="205">
         <v>0.92366895341794497</v>
       </c>
-      <c r="D33" s="136">
+      <c r="D33" s="138">
         <v>0.94611855796508304</v>
       </c>
-      <c r="E33" s="70">
+      <c r="E33" s="152">
         <v>0.95498447463069402</v>
       </c>
-      <c r="F33" s="136">
-        <v>0.92147883588139301</v>
-      </c>
-      <c r="G33" s="69">
-        <f t="shared" si="1"/>
-        <v>0.93656270547377873</v>
-      </c>
-      <c r="I33" s="169"/>
-      <c r="J33" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="K33" s="56">
-        <v>0.94133333333333302</v>
-      </c>
-      <c r="L33" s="60">
-        <v>0.94691356441715102</v>
-      </c>
-      <c r="M33" s="56">
-        <v>0.97502493880587304</v>
-      </c>
-      <c r="N33" s="84">
-        <v>0.960488422521524</v>
+      <c r="F33" s="183"/>
+      <c r="G33" s="202">
+        <f>AVERAGE(C33,D33,E33,F33)</f>
+        <v>0.94159066200457397</v>
+      </c>
+      <c r="I33" s="133" t="s">
+        <v>40</v>
+      </c>
+      <c r="J33" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="K33" s="147">
+        <v>0.93033333333333301</v>
+      </c>
+      <c r="L33" s="182">
+        <v>0.96681750536309896</v>
+      </c>
+      <c r="M33" s="147">
+        <v>0.93544479110025303</v>
+      </c>
+      <c r="N33" s="150">
+        <v>0.95037693946635804</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>8</v>
       </c>
-      <c r="B34" s="150" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" s="147">
+      <c r="B34" s="113" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="206">
         <v>0.92403795172563097</v>
       </c>
-      <c r="D34" s="137">
+      <c r="D34" s="207">
         <v>0.93904052682102801</v>
       </c>
-      <c r="E34" s="147">
+      <c r="E34" s="208">
         <v>0.94181503831139002</v>
       </c>
-      <c r="F34" s="137">
-        <v>0.94304824997875003</v>
-      </c>
-      <c r="G34" s="151">
-        <f t="shared" si="1"/>
-        <v>0.93698544170919984</v>
-      </c>
-      <c r="I34" s="169"/>
-      <c r="J34" s="86" t="s">
-        <v>37</v>
-      </c>
-      <c r="K34" s="92"/>
-      <c r="L34" s="93"/>
-      <c r="M34" s="92"/>
-      <c r="N34" s="94"/>
+      <c r="F34" s="183"/>
+      <c r="G34" s="209">
+        <f>AVERAGE(C34,D34,E34,F34)</f>
+        <v>0.93496450561934974</v>
+      </c>
+      <c r="I34" s="131"/>
+      <c r="J34" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="K34" s="151">
+        <v>0.93166666666666598</v>
+      </c>
+      <c r="L34" s="155">
+        <v>0.95452715920307196</v>
+      </c>
+      <c r="M34" s="151">
+        <v>0.94708254366936895</v>
+      </c>
+      <c r="N34" s="169">
+        <v>0.95050627178595104</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9</v>
       </c>
-      <c r="B35" s="141" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="70">
+      <c r="B35" s="107" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="199">
         <v>0.92966594521001</v>
       </c>
-      <c r="D35" s="136">
+      <c r="D35" s="200">
         <v>0.94811172337970895</v>
       </c>
-      <c r="E35" s="152">
+      <c r="E35" s="210">
         <v>0.960488422521524</v>
       </c>
-      <c r="F35" s="20">
-        <v>0.95167123552427801</v>
-      </c>
-      <c r="G35" s="99">
+      <c r="F35" s="189">
+        <v>0.95655542267451998</v>
+      </c>
+      <c r="G35" s="211">
         <f>AVERAGE(C35,D35,E35,F35)</f>
-        <v>0.94748433165888024</v>
-      </c>
-      <c r="I35" s="169"/>
-      <c r="J35" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="K35" s="92"/>
-      <c r="L35" s="93"/>
-      <c r="M35" s="92"/>
-      <c r="N35" s="94"/>
+        <v>0.94870537844644076</v>
+      </c>
+      <c r="I35" s="131"/>
+      <c r="J35" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" s="138">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="L35" s="155">
+        <v>0.96631050092293103</v>
+      </c>
+      <c r="M35" s="138">
+        <v>0.93679629830233901</v>
+      </c>
+      <c r="N35" s="154">
+        <v>0.95081201999177301</v>
+      </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>10</v>
       </c>
-      <c r="B36" s="141" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="155">
+      <c r="B36" s="107" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="212">
         <v>0.93380756718922198</v>
       </c>
-      <c r="D36" s="74">
+      <c r="D36" s="151">
         <v>0.95153501290619003</v>
       </c>
-      <c r="E36" s="70"/>
-      <c r="F36" s="136">
-        <v>0.948000240221335</v>
-      </c>
-      <c r="G36" s="69">
-        <f t="shared" ref="G36:G39" si="2">AVERAGE(C36,D36,E36,F36)</f>
-        <v>0.94444760677224904</v>
-      </c>
-      <c r="I36" s="169"/>
+      <c r="E36" s="166">
+        <v>0.96009563221816197</v>
+      </c>
+      <c r="F36" s="153">
+        <v>0.954781772342295</v>
+      </c>
+      <c r="G36" s="213">
+        <f>AVERAGE(C36,D36,E36,F36)</f>
+        <v>0.95005499616396727</v>
+      </c>
+      <c r="I36" s="131"/>
       <c r="J36" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="K36" s="92"/>
-      <c r="L36" s="93"/>
-      <c r="M36" s="92"/>
-      <c r="N36" s="94"/>
+        <v>31</v>
+      </c>
+      <c r="K36" s="183"/>
+      <c r="L36" s="184"/>
+      <c r="M36" s="183"/>
+      <c r="N36" s="185"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>11</v>
       </c>
-      <c r="B37" s="139" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="70">
+      <c r="B37" s="105" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="205">
         <v>0.92540717681603002</v>
       </c>
-      <c r="D37" s="136">
+      <c r="D37" s="153">
         <v>0.94430969519343799</v>
       </c>
-      <c r="E37" s="70"/>
-      <c r="F37" s="136">
-        <v>0.94945811231849997</v>
-      </c>
-      <c r="G37" s="69">
-        <f t="shared" si="2"/>
-        <v>0.93972499477598925</v>
-      </c>
-      <c r="I37" s="169"/>
+      <c r="E37" s="167">
+        <v>0.962621751359374</v>
+      </c>
+      <c r="F37" s="153">
+        <v>0.95274243556591998</v>
+      </c>
+      <c r="G37" s="202">
+        <f>AVERAGE(C37,D37,E37,F37)</f>
+        <v>0.94627026473369047</v>
+      </c>
+      <c r="I37" s="131"/>
       <c r="J37" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="K37" s="92"/>
-      <c r="L37" s="93"/>
-      <c r="M37" s="92"/>
-      <c r="N37" s="94" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="K37" s="183"/>
+      <c r="L37" s="184"/>
+      <c r="M37" s="183"/>
+      <c r="N37" s="185"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>12</v>
       </c>
-      <c r="B38" s="139" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="70">
+      <c r="B38" s="105" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="205">
         <v>0.926820944877769</v>
       </c>
-      <c r="D38" s="136">
+      <c r="D38" s="153">
         <v>0.91524186903115701</v>
       </c>
-      <c r="E38" s="70"/>
-      <c r="F38" s="136">
-        <v>0.93483765755288595</v>
-      </c>
-      <c r="G38" s="69">
-        <f t="shared" si="2"/>
-        <v>0.92563349048727062</v>
-      </c>
-      <c r="I38" s="170"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="71"/>
-      <c r="L38" s="83"/>
-      <c r="M38" s="71"/>
-      <c r="N38" s="85"/>
+      <c r="E38" s="166">
+        <v>0.95568813273184805</v>
+      </c>
+      <c r="F38" s="192">
+        <v>0.94923352876105405</v>
+      </c>
+      <c r="G38" s="202">
+        <f>AVERAGE(C38,D38,E38,F38)</f>
+        <v>0.936746118850457</v>
+      </c>
+      <c r="I38" s="131"/>
+      <c r="J38" s="186" t="s">
+        <v>24</v>
+      </c>
+      <c r="K38" s="187">
+        <v>0.94</v>
+      </c>
+      <c r="L38" s="188">
+        <v>0.962371595925259</v>
+      </c>
+      <c r="M38" s="189">
+        <v>0.951578111283513</v>
+      </c>
+      <c r="N38" s="190">
+        <v>0.95655542267451998</v>
+      </c>
     </row>
     <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>13</v>
       </c>
-      <c r="B39" s="142" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="83">
+      <c r="B39" s="108" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="214">
         <v>0.91222117035461403</v>
       </c>
-      <c r="D39" s="71">
+      <c r="D39" s="177">
         <v>0.949132760189906</v>
       </c>
-      <c r="E39" s="83"/>
-      <c r="F39" s="71">
-        <v>0.945670663459526</v>
-      </c>
-      <c r="G39" s="95">
-        <f t="shared" si="2"/>
-        <v>0.93567486466801542</v>
-      </c>
-      <c r="I39" s="168" t="s">
-        <v>40</v>
-      </c>
-      <c r="J39" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="K39" s="56">
-        <v>0.91366666666666596</v>
-      </c>
-      <c r="L39" s="138">
-        <v>0.95814644463200904</v>
-      </c>
-      <c r="M39" s="56">
-        <v>0.92440880347615895</v>
-      </c>
-      <c r="N39" s="84">
-        <v>0.94032543064146701</v>
+      <c r="E39" s="176">
+        <v>0.96020358147077001</v>
+      </c>
+      <c r="F39" s="215">
+        <v>0.956850923299568</v>
+      </c>
+      <c r="G39" s="216">
+        <f>AVERAGE(C39,D39,E39,F39)</f>
+        <v>0.94460210882871454</v>
+      </c>
+      <c r="I39" s="131"/>
+      <c r="J39" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="K39" s="153">
+        <v>0.93866666666666598</v>
+      </c>
+      <c r="L39" s="155">
+        <v>0.94064534425519297</v>
+      </c>
+      <c r="M39" s="151">
+        <v>0.969683980608673</v>
+      </c>
+      <c r="N39" s="156">
+        <v>0.954781772342295</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I40" s="169"/>
-      <c r="J40" s="82" t="s">
-        <v>30</v>
-      </c>
-      <c r="K40" s="54">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="L40" s="73">
-        <v>0.94553849671963197</v>
-      </c>
-      <c r="M40" s="54">
-        <v>0.94829895869616798</v>
-      </c>
-      <c r="N40" s="91">
-        <v>0.94621159827797796</v>
+      <c r="I40" s="131"/>
+      <c r="J40" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="K40" s="153">
+        <v>0.93433333333333302</v>
+      </c>
+      <c r="L40" s="152">
+        <v>0.96014970108411501</v>
+      </c>
+      <c r="M40" s="153">
+        <v>0.94685932478122903</v>
+      </c>
+      <c r="N40" s="156">
+        <v>0.95274243556591998</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="140"/>
+      <c r="B41" s="106"/>
       <c r="C41" s="43"/>
       <c r="D41" s="43"/>
       <c r="E41" s="47"/>
       <c r="F41" s="47"/>
       <c r="G41" s="47"/>
-      <c r="I41" s="169"/>
-      <c r="J41" s="78" t="s">
-        <v>33</v>
-      </c>
-      <c r="K41" s="63">
-        <v>0.91899999999999904</v>
-      </c>
-      <c r="L41" s="73">
-        <v>0.94124794486665697</v>
-      </c>
-      <c r="M41" s="63">
-        <v>0.94553388433052599</v>
-      </c>
-      <c r="N41" s="89">
-        <v>0.94265481086242897</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I42" s="169"/>
-      <c r="J42" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="K42" s="63">
-        <v>0.91899999999999904</v>
-      </c>
-      <c r="L42" s="73">
-        <v>0.94963155161494806</v>
-      </c>
-      <c r="M42" s="63">
-        <v>0.93824108603561296</v>
-      </c>
-      <c r="N42" s="89">
-        <v>0.94304824997875003</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I43" s="169"/>
-      <c r="J43" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="K43" s="49">
-        <v>0.88866666666666605</v>
-      </c>
-      <c r="L43" s="73">
-        <v>0.92198048434218205</v>
-      </c>
-      <c r="M43" s="63">
-        <v>0.92655628502728204</v>
-      </c>
-      <c r="N43" s="88">
-        <v>0.92147883588139301</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I44" s="169"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="90"/>
-      <c r="L44" s="70"/>
-      <c r="M44" s="90"/>
-      <c r="N44" s="87"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I41" s="131"/>
+      <c r="J41" s="100" t="s">
+        <v>35</v>
+      </c>
+      <c r="K41" s="151">
+        <v>0.94</v>
+      </c>
+      <c r="L41" s="191">
+        <v>0.96723665991626695</v>
+      </c>
+      <c r="M41" s="192">
+        <v>0.94738578696838205</v>
+      </c>
+      <c r="N41" s="193">
+        <v>0.956850923299568</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I42" s="134"/>
+      <c r="J42" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="K42" s="162">
+        <v>0.93166666666666598</v>
+      </c>
+      <c r="L42" s="194">
+        <v>0.93069898718275901</v>
+      </c>
+      <c r="M42" s="195">
+        <v>0.96898477316130405</v>
+      </c>
+      <c r="N42" s="196">
+        <v>0.94923352876105405</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E45" s="14"/>
-      <c r="I45" s="169"/>
-      <c r="J45" s="98" t="s">
-        <v>24</v>
-      </c>
-      <c r="K45" s="24">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="L45" s="159">
-        <v>0.94774151470795298</v>
-      </c>
-      <c r="M45" s="158">
-        <v>0.95603291396641799</v>
-      </c>
-      <c r="N45" s="20">
-        <v>0.95167123552427801</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I45" s="217"/>
+      <c r="J45" s="218" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E46" s="14"/>
-      <c r="I46" s="169"/>
-      <c r="J46" s="86" t="s">
-        <v>37</v>
-      </c>
-      <c r="K46" s="96">
-        <v>0.92533333333333301</v>
-      </c>
-      <c r="L46" s="65">
-        <v>0.96202419744587098</v>
-      </c>
-      <c r="M46" s="49">
-        <v>0.93519467031457704</v>
-      </c>
-      <c r="N46" s="52">
-        <v>0.948000240221335</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I46" s="219"/>
+      <c r="J46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="14"/>
-      <c r="I47" s="169"/>
-      <c r="J47" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="K47" s="96">
-        <v>0.92833333333333301</v>
-      </c>
-      <c r="L47" s="51">
-        <v>0.95202520822885595</v>
-      </c>
-      <c r="M47" s="49">
-        <v>0.947454591393594</v>
-      </c>
-      <c r="N47" s="52">
-        <v>0.94945811231849997</v>
+      <c r="I47" s="220"/>
+      <c r="J47" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E48" s="14"/>
-      <c r="I48" s="169"/>
-      <c r="J48" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="K48" s="96">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="L48" s="133">
-        <v>0.93539714008536201</v>
-      </c>
-      <c r="M48" s="134">
-        <v>0.95746271297063801</v>
-      </c>
-      <c r="N48" s="132">
-        <v>0.945670663459526</v>
-      </c>
-    </row>
-    <row r="49" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E49" s="128"/>
-      <c r="I49" s="169"/>
-      <c r="J49" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="K49" s="96">
-        <v>0.91099999999999903</v>
-      </c>
-      <c r="L49" s="73">
-        <v>0.90790109724912105</v>
-      </c>
-      <c r="M49" s="54">
-        <v>0.96444487236179499</v>
-      </c>
-      <c r="N49" s="52">
-        <v>0.93483765755288595</v>
-      </c>
-    </row>
-    <row r="50" spans="5:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I50" s="170"/>
-      <c r="J50" s="38"/>
-      <c r="K50" s="97"/>
-      <c r="L50" s="83"/>
-      <c r="M50" s="71"/>
-      <c r="N50" s="95"/>
+      <c r="I48" s="221" t="s">
+        <v>18</v>
+      </c>
+      <c r="J48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E49" s="97"/>
+      <c r="I49" s="222" t="s">
+        <v>18</v>
+      </c>
+      <c r="J49" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="I39:I50"/>
-    <mergeCell ref="I27:I38"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="B8:B12"/>
-    <mergeCell ref="I3:I14"/>
-    <mergeCell ref="I15:I26"/>
+    <mergeCell ref="I3:I12"/>
+    <mergeCell ref="I13:I22"/>
+    <mergeCell ref="I23:I32"/>
+    <mergeCell ref="I33:I42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5752,10 +5936,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G13"/>
+  <dimension ref="B2:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5768,177 +5952,293 @@
     <col min="7" max="7" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="168" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="36" t="s">
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="114"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="142" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="87">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="E3" s="88">
+        <v>0.83380446160172395</v>
+      </c>
+      <c r="F3" s="87">
+        <v>0.822946213095609</v>
+      </c>
+      <c r="G3" s="89">
+        <v>0.82443696037685399</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="143"/>
+      <c r="C4" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="73">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="E4" s="140">
+        <v>0.88455725174062005</v>
+      </c>
+      <c r="F4" s="73">
+        <v>0.88943449794617901</v>
+      </c>
+      <c r="G4" s="75">
+        <v>0.88272122487528404</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="143"/>
+      <c r="C5" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="83">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="E5" s="140">
+        <v>0.94774151470795298</v>
+      </c>
+      <c r="F5" s="83">
+        <v>0.95603291396641799</v>
+      </c>
+      <c r="G5" s="84">
+        <v>0.95167123552427801</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="143"/>
+      <c r="C6" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="70">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="E6" s="141">
+        <v>0.93529471319514301</v>
+      </c>
+      <c r="F6" s="70">
+        <v>0.84111573320072097</v>
+      </c>
+      <c r="G6" s="72">
+        <v>0.87920035047497902</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="144"/>
+      <c r="C7" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="92">
+        <v>0.91366666666666596</v>
+      </c>
+      <c r="E7" s="96">
+        <v>0.95814644463200904</v>
+      </c>
+      <c r="F7" s="92">
+        <v>0.92440880347615895</v>
+      </c>
+      <c r="G7" s="95">
+        <v>0.94032543064146701</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="114"/>
+    </row>
+    <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="135" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="56">
-        <v>0.93033333333333301</v>
-      </c>
-      <c r="E2" s="138">
-        <v>0.96681750536309896</v>
-      </c>
-      <c r="F2" s="56">
-        <v>0.93544479110025303</v>
-      </c>
-      <c r="G2" s="84">
-        <v>0.95037693946635804</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="169"/>
-      <c r="C3" s="82" t="s">
+      <c r="D11" s="55">
+        <v>0.91366666666666596</v>
+      </c>
+      <c r="E11" s="104">
+        <v>0.95814644463200904</v>
+      </c>
+      <c r="F11" s="55">
+        <v>0.92440880347615895</v>
+      </c>
+      <c r="G11" s="63">
+        <v>0.94032543064146701</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="136"/>
+      <c r="C12" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="94"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="169"/>
-      <c r="C4" s="78" t="s">
+      <c r="D12" s="54">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="E12" s="60">
+        <v>0.94553849671963197</v>
+      </c>
+      <c r="F12" s="54">
+        <v>0.94829895869616798</v>
+      </c>
+      <c r="G12" s="67">
+        <v>0.94621159827797796</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="136"/>
+      <c r="C13" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="92"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="94"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="169"/>
-      <c r="C5" s="37" t="s">
+      <c r="D13" s="58">
+        <v>0.91899999999999904</v>
+      </c>
+      <c r="E13" s="60">
+        <v>0.94124794486665697</v>
+      </c>
+      <c r="F13" s="58">
+        <v>0.94553388433052599</v>
+      </c>
+      <c r="G13" s="66">
+        <v>0.94265481086242897</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="136"/>
+      <c r="C14" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="92"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="94"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="169"/>
-      <c r="C6" s="37" t="s">
+      <c r="D14" s="58">
+        <v>0.91899999999999904</v>
+      </c>
+      <c r="E14" s="60">
+        <v>0.94963155161494806</v>
+      </c>
+      <c r="F14" s="58">
+        <v>0.93824108603561296</v>
+      </c>
+      <c r="G14" s="66">
+        <v>0.94304824997875003</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="136"/>
+      <c r="C15" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="92"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="94"/>
-    </row>
-    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="169"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="160"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="160"/>
-      <c r="G7" s="87"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="169"/>
-      <c r="C8" s="98" t="s">
+      <c r="D15" s="49">
+        <v>0.88866666666666605</v>
+      </c>
+      <c r="E15" s="60">
+        <v>0.92198048434218205</v>
+      </c>
+      <c r="F15" s="58">
+        <v>0.92655628502728204</v>
+      </c>
+      <c r="G15" s="65">
+        <v>0.92147883588139301</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="136"/>
+      <c r="C16" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="24">
-        <v>0.94</v>
-      </c>
-      <c r="E8" s="159">
-        <v>0.962371595925259</v>
-      </c>
-      <c r="F8" s="158">
-        <v>0.951578111283513</v>
-      </c>
-      <c r="G8" s="20">
-        <v>0.95655542267451998</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="169"/>
-      <c r="C9" s="86" t="s">
+      <c r="D16" s="115">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="E16" s="116">
+        <v>0.94774151470795298</v>
+      </c>
+      <c r="F16" s="117">
+        <v>0.95603291396641799</v>
+      </c>
+      <c r="G16" s="118">
+        <v>0.95167123552427801</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="136"/>
+      <c r="C17" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="96">
-        <v>0.93866666666666598</v>
-      </c>
-      <c r="E9" s="73">
-        <v>0.94064534425519297</v>
-      </c>
-      <c r="F9" s="63">
-        <v>0.969683980608673</v>
-      </c>
-      <c r="G9" s="52">
-        <v>0.954781772342295</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="169"/>
-      <c r="C10" s="78" t="s">
+      <c r="D17" s="68">
+        <v>0.92533333333333301</v>
+      </c>
+      <c r="E17" s="59">
+        <v>0.96202419744587098</v>
+      </c>
+      <c r="F17" s="49">
+        <v>0.93519467031457704</v>
+      </c>
+      <c r="G17" s="52">
+        <v>0.948000240221335</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="136"/>
+      <c r="C18" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="96">
-        <v>0.93433333333333302</v>
-      </c>
-      <c r="E10" s="51">
-        <v>0.96014970108411501</v>
-      </c>
-      <c r="F10" s="49">
-        <v>0.94685932478122903</v>
-      </c>
-      <c r="G10" s="52">
-        <v>0.95274243556591998</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="169"/>
-      <c r="C11" s="37" t="s">
+      <c r="D18" s="68">
+        <v>0.92833333333333301</v>
+      </c>
+      <c r="E18" s="51">
+        <v>0.95202520822885595</v>
+      </c>
+      <c r="F18" s="49">
+        <v>0.947454591393594</v>
+      </c>
+      <c r="G18" s="52">
+        <v>0.94945811231849997</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="136"/>
+      <c r="C19" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="161">
-        <v>0.94</v>
-      </c>
-      <c r="E11" s="162">
-        <v>0.96723665991626695</v>
-      </c>
-      <c r="F11" s="163">
-        <v>0.94738578696838205</v>
-      </c>
-      <c r="G11" s="164">
-        <v>0.956850923299568</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="169"/>
-      <c r="C12" s="37" t="s">
+      <c r="D19" s="68">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="E19" s="102">
+        <v>0.93539714008536201</v>
+      </c>
+      <c r="F19" s="103">
+        <v>0.95746271297063801</v>
+      </c>
+      <c r="G19" s="101">
+        <v>0.945670663459526</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="137"/>
+      <c r="C20" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="96">
-        <v>0.93166666666666598</v>
-      </c>
-      <c r="E12" s="133">
-        <v>0.93069898718275901</v>
-      </c>
-      <c r="F12" s="134">
-        <v>0.96898477316130405</v>
-      </c>
-      <c r="G12" s="132">
-        <v>0.94923352876105405</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="170"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="95"/>
+      <c r="D20" s="119">
+        <v>0.91099999999999903</v>
+      </c>
+      <c r="E20" s="120">
+        <v>0.90790109724912105</v>
+      </c>
+      <c r="F20" s="121">
+        <v>0.96444487236179499</v>
+      </c>
+      <c r="G20" s="122">
+        <v>0.93483765755288595</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:B13"/>
+  <mergeCells count="2">
+    <mergeCell ref="B11:B20"/>
+    <mergeCell ref="B3:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>